<commit_message>
Modified modules locaiton and table representation
</commit_message>
<xml_diff>
--- a/08_Milling_OT.xlsx
+++ b/08_Milling_OT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h.kostov\Documents\CustomDocuments\TMP\PythonScriptTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uKBo\OneDrive\Documents\PythonScriptTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EFD1C95-2835-4F20-AD5D-915E72320B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DCF2BB-7990-45AA-B72C-373AE0C1AD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{5A042C1D-8242-4401-85C6-5A82A7DD8CAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5A042C1D-8242-4401-85C6-5A82A7DD8CAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
   <customWorkbookViews>
     <customWorkbookView name="Someone - Personal View" guid="{801DBE99-3CFE-4EBC-BEBB-E522DC1A6736}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
-  <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
-  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>PART NUMBER</t>
   </si>
@@ -443,39 +440,6 @@
   <si>
     <t>Общи площи/м2</t>
   </si>
-  <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>AISI 304 
-30x20(шина)</t>
-  </si>
-  <si>
-    <t>AISI 304 ТР.Ш 
-60x60x3</t>
-  </si>
-  <si>
-    <t>AISI 304-
-55x20(шина)</t>
-  </si>
-  <si>
-    <t>POLIURETHANE L-
-1312mm</t>
-  </si>
-  <si>
-    <t>POM-
-C/D80(бял)</t>
-  </si>
-  <si>
-    <t>РОМ-
-C/D40/D20-бял</t>
-  </si>
-  <si>
-    <t>Sum of Общи площи/м2</t>
-  </si>
-  <si>
-    <t>Sum of Общи дължини на профили/мм</t>
-  </si>
 </sst>
 </file>
 
@@ -484,7 +448,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -615,14 +579,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" pivotButton="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -630,184 +586,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -818,706 +597,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Someone" refreshedDate="45552.563274537039" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="15" xr:uid="{D0B85148-FAB0-45ED-A1CD-76B215DD4CA2}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:X16" sheet="Sheet1"/>
-  </cacheSource>
-  <cacheFields count="24">
-    <cacheField name="PART NUMBER" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="11968" maxValue="23974"/>
-    </cacheField>
-    <cacheField name="DESCRIPTION" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="QTY." numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
-    </cacheField>
-    <cacheField name="Material" numFmtId="0">
-      <sharedItems count="13">
-        <s v="S235JR"/>
-        <s v="S235JR "/>
-        <s v="AISI 304-_x000a_55x20(шина)"/>
-        <s v="AISI 304 _x000a_30x20(шина)"/>
-        <s v="AISI 304 D12/h9"/>
-        <s v="AISI 304/M16"/>
-        <s v="AISI 304/M3"/>
-        <s v="AISI 304/M8"/>
-        <s v="POM-_x000a_C/D80(бял)"/>
-        <s v="РОМ-_x000a_C/D40/D20-бял"/>
-        <s v="AISI 304 ТР.Ш _x000a_60x60x3"/>
-        <s v="AISI 304/D4"/>
-        <s v="POLIURETHANE L-_x000a_1312mm"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Sheeet metal _x000a_thickness" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="12" maxValue="60" count="4">
-        <n v="12"/>
-        <n v="60"/>
-        <n v="20"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="CAD_length/mm" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="20" maxValue="17470"/>
-    </cacheField>
-    <cacheField name="Surface _x000a_area/m2" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.01" maxValue="0.25"/>
-    </cacheField>
-    <cacheField name="Cad_perimeter/mm" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="600" maxValue="2597"/>
-    </cacheField>
-    <cacheField name="Processing" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Files" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Material 1" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="CAD_length 1/mm" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Material 2" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="CAD_length 2/mm" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Material 3" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="CAD_length 3/mm" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="TETAMAT code" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="11968" maxValue="21669"/>
-    </cacheField>
-    <cacheField name="Producer" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Producer code" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Supplier" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="CAD_ZONE " numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Cad weight/g" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="4.51" maxValue="91069.930999999997"/>
-    </cacheField>
-    <cacheField name="Общи дължини на профили/мм" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="17470"/>
-    </cacheField>
-    <cacheField name="Общи площи/м2" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.5"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="15">
-  <r>
-    <n v="21683"/>
-    <s v="Плоча"/>
-    <n v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <m/>
-    <n v="0.01"/>
-    <n v="600"/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="1017.748"/>
-    <n v="0"/>
-    <n v="0.02"/>
-  </r>
-  <r>
-    <n v="23956"/>
-    <s v="Плоча"/>
-    <n v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <m/>
-    <n v="0.25"/>
-    <n v="2597"/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="21657"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="115.986"/>
-    <n v="0"/>
-    <n v="0.5"/>
-  </r>
-  <r>
-    <n v="19170"/>
-    <s v="Планка"/>
-    <n v="8"/>
-    <x v="2"/>
-    <x v="2"/>
-    <n v="100"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="19170"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="713.38"/>
-    <n v="800"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="21686"/>
-    <s v="Планка"/>
-    <n v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <n v="120"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="19170"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="747.92"/>
-    <n v="240"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <s v="016386.01.00"/>
-    <s v="Планка"/>
-    <n v="10"/>
-    <x v="3"/>
-    <x v="3"/>
-    <n v="208"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="967.86"/>
-    <n v="2080"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="23968"/>
-    <s v="Ос"/>
-    <n v="1"/>
-    <x v="4"/>
-    <x v="3"/>
-    <n v="500"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="452.1"/>
-    <n v="500"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="21659"/>
-    <s v="Шпилка"/>
-    <n v="2"/>
-    <x v="5"/>
-    <x v="3"/>
-    <n v="185"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="21659"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="297.18599999999998"/>
-    <n v="370"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="23974"/>
-    <s v="Шпилка M3x80"/>
-    <n v="2"/>
-    <x v="6"/>
-    <x v="3"/>
-    <n v="80"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="4.51"/>
-    <n v="160"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="23949"/>
-    <s v="Шпилка "/>
-    <n v="2"/>
-    <x v="7"/>
-    <x v="3"/>
-    <n v="40"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="14.94"/>
-    <n v="80"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="21669"/>
-    <s v="Шайба"/>
-    <n v="2"/>
-    <x v="8"/>
-    <x v="3"/>
-    <n v="20"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="21669"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="97.656999999999996"/>
-    <n v="40"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="21660"/>
-    <s v="Втулка"/>
-    <n v="2"/>
-    <x v="9"/>
-    <x v="3"/>
-    <n v="115"/>
-    <m/>
-    <m/>
-    <s v="Milling"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="21660"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="110.553"/>
-    <n v="230"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="23927"/>
-    <s v="Рамка"/>
-    <n v="1"/>
-    <x v="10"/>
-    <x v="3"/>
-    <n v="17470"/>
-    <m/>
-    <m/>
-    <s v="Saw_cutting"/>
-    <s v="DRAWING"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="91069.930999999997"/>
-    <n v="17470"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <s v="4.2 TETAMAT  CABLE _x000a_TRAY"/>
-    <s v="TETAMAT  CABLE TRAY-_x000a_500мм"/>
-    <n v="1"/>
-    <x v="11"/>
-    <x v="3"/>
-    <n v="2500"/>
-    <m/>
-    <m/>
-    <s v="Saw_cutting"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="4.2 TETAMAT  _x000a_CABLE TRAY"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="32.119"/>
-    <n v="2500"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <s v="4.2 TETAMAT  CABLE _x000a_TRAY"/>
-    <s v="TETAMAT  CABLE TRAY-_x000a_800мм"/>
-    <n v="1"/>
-    <x v="11"/>
-    <x v="3"/>
-    <n v="4200"/>
-    <m/>
-    <m/>
-    <s v="Saw_cutting"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <s v="4.2 TETAMAT  _x000a_CABLE TRAY"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="50.673000000000002"/>
-    <n v="4200"/>
-    <n v="0"/>
-  </r>
-  <r>
-    <n v="11968"/>
-    <s v="Полиуретанов _x000a_уплътнител "/>
-    <n v="1"/>
-    <x v="12"/>
-    <x v="3"/>
-    <n v="1312"/>
-    <m/>
-    <m/>
-    <s v="Saw_cutting"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <n v="11968"/>
-    <s v="РОДОП"/>
-    <s v="480/6x20/"/>
-    <s v="РОДОП"/>
-    <s v="CAD_zone-2"/>
-    <n v="105.336"/>
-    <n v="1312"/>
-    <n v="0"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D3209D2-66DF-4A96-A877-8CEB5AFE1B5C}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="Z1:AB17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="24">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="14">
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="10"/>
-        <item x="2"/>
-        <item sd="0" x="11"/>
-        <item sd="0" x="5"/>
-        <item sd="0" x="6"/>
-        <item sd="0" x="7"/>
-        <item sd="0" x="12"/>
-        <item sd="0" x="8"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item sd="0" x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="3"/>
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="16">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Sum of Общи площи/м2" fld="23" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Общи дължини на профили/мм" fld="22" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="8">
-    <format dxfId="7">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="3" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="4" count="1">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="3" count="1" selected="0">
-            <x v="10"/>
-          </reference>
-          <reference field="4" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="3" count="1" selected="0">
-            <x v="11"/>
-          </reference>
-          <reference field="4" count="1">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="2">
-            <x v="0"/>
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1837,44 +916,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BB7FF8-B958-4DD7-8A02-EE574F45E3E9}">
-  <dimension ref="A1:AC175"/>
+  <dimension ref="A1:Z175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="9" style="3"/>
-    <col min="26" max="26" width="26.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="9" style="3"/>
+    <col min="26" max="26" width="33" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="72">
+    <row r="1" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1947,19 +1024,10 @@
       <c r="X1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB1" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC1"/>
-    </row>
-    <row r="2" spans="1:29" ht="26.4">
-      <c r="A2" s="15">
+      <c r="Z1"/>
+    </row>
+    <row r="2" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
         <v>21683</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2009,19 +1077,10 @@
         <f>C2*G2</f>
         <v>0.02</v>
       </c>
-      <c r="Z2" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA2" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="12">
-        <v>2080</v>
-      </c>
-      <c r="AC2"/>
-    </row>
-    <row r="3" spans="1:29" ht="26.4">
-      <c r="A3" s="15">
+      <c r="Z2"/>
+    </row>
+    <row r="3" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
         <v>23956</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2073,19 +1132,10 @@
         <f t="shared" ref="X3:X16" si="1">C3*G3</f>
         <v>0.5</v>
       </c>
-      <c r="Z3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="12">
-        <v>500</v>
-      </c>
-      <c r="AC3"/>
-    </row>
-    <row r="4" spans="1:29" ht="26.4">
-      <c r="A4" s="15">
+      <c r="Z3"/>
+    </row>
+    <row r="4" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>19170</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2135,19 +1185,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z4" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA4" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="12">
-        <v>17470</v>
-      </c>
-      <c r="AC4"/>
-    </row>
-    <row r="5" spans="1:29" ht="26.4">
-      <c r="A5" s="15">
+      <c r="Z4"/>
+    </row>
+    <row r="5" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>21686</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2197,19 +1238,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z5" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA5" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="12">
-        <v>1040</v>
-      </c>
-      <c r="AC5"/>
-    </row>
-    <row r="6" spans="1:29" ht="26.4">
-      <c r="A6" s="15" t="s">
+      <c r="Z5"/>
+    </row>
+    <row r="6" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2255,19 +1287,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z6" s="14">
-        <v>20</v>
-      </c>
-      <c r="AA6" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="12">
-        <v>1040</v>
-      </c>
-      <c r="AC6"/>
-    </row>
-    <row r="7" spans="1:29" ht="26.4">
-      <c r="A7" s="15">
+      <c r="Z6"/>
+    </row>
+    <row r="7" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
         <v>23968</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2313,19 +1336,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA7" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="12">
-        <v>6700</v>
-      </c>
-      <c r="AC7"/>
-    </row>
-    <row r="8" spans="1:29" ht="26.4">
-      <c r="A8" s="15">
+      <c r="Z7"/>
+    </row>
+    <row r="8" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>21659</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2373,19 +1387,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA8" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="12">
-        <v>370</v>
-      </c>
-      <c r="AC8"/>
-    </row>
-    <row r="9" spans="1:29" ht="26.4">
-      <c r="A9" s="15">
+      <c r="Z8"/>
+    </row>
+    <row r="9" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
         <v>23974</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -2431,19 +1436,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA9" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="12">
-        <v>160</v>
-      </c>
-      <c r="AC9"/>
-    </row>
-    <row r="10" spans="1:29" ht="26.4">
-      <c r="A10" s="15">
+      <c r="Z9"/>
+    </row>
+    <row r="10" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
         <v>23949</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -2489,19 +1485,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z10" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA10" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="12">
-        <v>80</v>
-      </c>
-      <c r="AC10"/>
-    </row>
-    <row r="11" spans="1:29" ht="26.4">
-      <c r="A11" s="15">
+      <c r="Z10"/>
+    </row>
+    <row r="11" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
         <v>21669</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -2549,19 +1536,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z11" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="AA11" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="12">
-        <v>1312</v>
-      </c>
-      <c r="AC11"/>
-    </row>
-    <row r="12" spans="1:29" ht="39.6">
-      <c r="A12" s="15">
+      <c r="Z11"/>
+    </row>
+    <row r="12" spans="1:26" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
         <v>21660</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -2609,19 +1587,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA12" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="12">
-        <v>40</v>
-      </c>
-      <c r="AC12"/>
-    </row>
-    <row r="13" spans="1:29" ht="26.4">
-      <c r="A13" s="15">
+      <c r="Z12"/>
+    </row>
+    <row r="13" spans="1:26" ht="27" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>23927</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -2667,19 +1636,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z13" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA13" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AB13" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC13"/>
-    </row>
-    <row r="14" spans="1:29" ht="66">
-      <c r="A14" s="15" t="s">
+      <c r="Z13"/>
+    </row>
+    <row r="14" spans="1:26" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -2725,19 +1685,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z14" s="14">
-        <v>12</v>
-      </c>
-      <c r="AA14" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="AB14" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC14"/>
-    </row>
-    <row r="15" spans="1:29" ht="66">
-      <c r="A15" s="15" t="s">
+      <c r="Z14"/>
+    </row>
+    <row r="15" spans="1:26" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -2783,19 +1734,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z15" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA15" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AB15" s="12">
-        <v>0</v>
-      </c>
-      <c r="AC15"/>
-    </row>
-    <row r="16" spans="1:29" ht="39.6">
-      <c r="A16" s="15">
+      <c r="Z15"/>
+    </row>
+    <row r="16" spans="1:26" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>11968</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2849,17 +1791,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z16" s="14">
-        <v>60</v>
-      </c>
-      <c r="AA16" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="AB16" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="14.4">
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2882,17 +1815,8 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="Z17" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA17" s="12">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="12">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="14.4">
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2915,11 +1839,8 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
-      <c r="Z18"/>
-      <c r="AA18"/>
-      <c r="AB18"/>
-    </row>
-    <row r="19" spans="1:28" ht="14.4">
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2942,11 +1863,8 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-      <c r="Z19"/>
-      <c r="AA19"/>
-      <c r="AB19"/>
-    </row>
-    <row r="20" spans="1:28" ht="14.4">
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2969,11 +1887,8 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
-      <c r="Z20"/>
-      <c r="AA20"/>
-      <c r="AB20"/>
-    </row>
-    <row r="21" spans="1:28" ht="14.4">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2996,11 +1911,8 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
-      <c r="Z21"/>
-      <c r="AA21"/>
-      <c r="AB21"/>
-    </row>
-    <row r="22" spans="1:28" ht="14.4">
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -3023,11 +1935,8 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
-      <c r="Z22"/>
-      <c r="AA22"/>
-      <c r="AB22"/>
-    </row>
-    <row r="23" spans="1:28" ht="14.4">
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -3050,11 +1959,8 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
-      <c r="Z23"/>
-      <c r="AA23"/>
-      <c r="AB23"/>
-    </row>
-    <row r="24" spans="1:28" ht="14.4">
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -3077,11 +1983,8 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
-      <c r="Z24"/>
-      <c r="AA24"/>
-      <c r="AB24"/>
-    </row>
-    <row r="25" spans="1:28" ht="14.4">
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -3104,11 +2007,8 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
-      <c r="Z25"/>
-      <c r="AA25"/>
-      <c r="AB25"/>
-    </row>
-    <row r="26" spans="1:28" ht="14.4">
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -3131,11 +2031,8 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
-      <c r="Z26"/>
-      <c r="AA26"/>
-      <c r="AB26"/>
-    </row>
-    <row r="27" spans="1:28" ht="14.4">
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -3158,11 +2055,8 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
-      <c r="Z27"/>
-      <c r="AA27"/>
-      <c r="AB27"/>
-    </row>
-    <row r="28" spans="1:28" ht="14.4">
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -3185,11 +2079,8 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-      <c r="Z28"/>
-      <c r="AA28"/>
-      <c r="AB28"/>
-    </row>
-    <row r="29" spans="1:28">
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -3213,7 +2104,7 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -3237,7 +2128,7 @@
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -3261,7 +2152,7 @@
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -3285,7 +2176,7 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3309,7 +2200,7 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3333,7 +2224,7 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3357,7 +2248,7 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3381,7 +2272,7 @@
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3405,7 +2296,7 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3429,7 +2320,7 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3453,7 +2344,7 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3477,7 +2368,7 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
     </row>
-    <row r="41" spans="1:22">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3501,7 +2392,7 @@
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
     </row>
-    <row r="42" spans="1:22">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3525,7 +2416,7 @@
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
     </row>
-    <row r="43" spans="1:22">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3549,7 +2440,7 @@
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3573,7 +2464,7 @@
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3597,7 +2488,7 @@
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3621,7 +2512,7 @@
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3645,7 +2536,7 @@
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3669,7 +2560,7 @@
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
     </row>
-    <row r="49" spans="1:22">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3693,7 +2584,7 @@
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
     </row>
-    <row r="50" spans="1:22">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3717,7 +2608,7 @@
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
     </row>
-    <row r="51" spans="1:22">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3741,7 +2632,7 @@
       <c r="U51" s="1"/>
       <c r="V51" s="1"/>
     </row>
-    <row r="52" spans="1:22">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3765,7 +2656,7 @@
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
     </row>
-    <row r="53" spans="1:22">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3789,7 +2680,7 @@
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
     </row>
-    <row r="54" spans="1:22">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3813,7 +2704,7 @@
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
     </row>
-    <row r="55" spans="1:22">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3837,7 +2728,7 @@
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
     </row>
-    <row r="56" spans="1:22">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3861,7 +2752,7 @@
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
     </row>
-    <row r="57" spans="1:22">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3885,7 +2776,7 @@
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
     </row>
-    <row r="58" spans="1:22">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3909,7 +2800,7 @@
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
     </row>
-    <row r="59" spans="1:22">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3933,7 +2824,7 @@
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
     </row>
-    <row r="60" spans="1:22">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3957,7 +2848,7 @@
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
     </row>
-    <row r="61" spans="1:22">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3981,7 +2872,7 @@
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
     </row>
-    <row r="62" spans="1:22">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4005,7 +2896,7 @@
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
     </row>
-    <row r="63" spans="1:22">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4029,7 +2920,7 @@
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
     </row>
-    <row r="64" spans="1:22">
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4053,7 +2944,7 @@
       <c r="U64" s="1"/>
       <c r="V64" s="1"/>
     </row>
-    <row r="65" spans="1:22">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4077,7 +2968,7 @@
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
     </row>
-    <row r="66" spans="1:22">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4101,7 +2992,7 @@
       <c r="U66" s="1"/>
       <c r="V66" s="1"/>
     </row>
-    <row r="67" spans="1:22">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4125,7 +3016,7 @@
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4149,7 +3040,7 @@
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4173,7 +3064,7 @@
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4197,7 +3088,7 @@
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4221,7 +3112,7 @@
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4245,7 +3136,7 @@
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4269,7 +3160,7 @@
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4293,7 +3184,7 @@
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4317,7 +3208,7 @@
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
     </row>
-    <row r="76" spans="1:22">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4341,7 +3232,7 @@
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
     </row>
-    <row r="77" spans="1:22">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4365,7 +3256,7 @@
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
     </row>
-    <row r="78" spans="1:22">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4389,7 +3280,7 @@
       <c r="U78" s="1"/>
       <c r="V78" s="1"/>
     </row>
-    <row r="79" spans="1:22">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4413,7 +3304,7 @@
       <c r="U79" s="1"/>
       <c r="V79" s="1"/>
     </row>
-    <row r="80" spans="1:22">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4437,7 +3328,7 @@
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
     </row>
-    <row r="81" spans="1:22">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4461,7 +3352,7 @@
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
     </row>
-    <row r="82" spans="1:22">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4485,7 +3376,7 @@
       <c r="U82" s="1"/>
       <c r="V82" s="1"/>
     </row>
-    <row r="83" spans="1:22">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4509,7 +3400,7 @@
       <c r="U83" s="1"/>
       <c r="V83" s="1"/>
     </row>
-    <row r="84" spans="1:22">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4533,7 +3424,7 @@
       <c r="U84" s="1"/>
       <c r="V84" s="1"/>
     </row>
-    <row r="85" spans="1:22">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -4557,7 +3448,7 @@
       <c r="U85" s="1"/>
       <c r="V85" s="1"/>
     </row>
-    <row r="86" spans="1:22">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -4581,7 +3472,7 @@
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
     </row>
-    <row r="87" spans="1:22">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -4605,7 +3496,7 @@
       <c r="U87" s="1"/>
       <c r="V87" s="1"/>
     </row>
-    <row r="88" spans="1:22">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -4629,7 +3520,7 @@
       <c r="U88" s="1"/>
       <c r="V88" s="1"/>
     </row>
-    <row r="89" spans="1:22">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -4653,7 +3544,7 @@
       <c r="U89" s="1"/>
       <c r="V89" s="1"/>
     </row>
-    <row r="90" spans="1:22">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -4677,7 +3568,7 @@
       <c r="U90" s="1"/>
       <c r="V90" s="1"/>
     </row>
-    <row r="91" spans="1:22">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -4701,7 +3592,7 @@
       <c r="U91" s="1"/>
       <c r="V91" s="1"/>
     </row>
-    <row r="92" spans="1:22">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -4725,7 +3616,7 @@
       <c r="U92" s="1"/>
       <c r="V92" s="1"/>
     </row>
-    <row r="93" spans="1:22">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -4749,7 +3640,7 @@
       <c r="U93" s="1"/>
       <c r="V93" s="1"/>
     </row>
-    <row r="94" spans="1:22">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -4773,7 +3664,7 @@
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
     </row>
-    <row r="95" spans="1:22">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -4797,7 +3688,7 @@
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
     </row>
-    <row r="96" spans="1:22">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -4821,7 +3712,7 @@
       <c r="U96" s="1"/>
       <c r="V96" s="1"/>
     </row>
-    <row r="97" spans="1:22">
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -4845,7 +3736,7 @@
       <c r="U97" s="1"/>
       <c r="V97" s="1"/>
     </row>
-    <row r="98" spans="1:22">
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -4869,7 +3760,7 @@
       <c r="U98" s="1"/>
       <c r="V98" s="1"/>
     </row>
-    <row r="99" spans="1:22">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -4893,7 +3784,7 @@
       <c r="U99" s="1"/>
       <c r="V99" s="1"/>
     </row>
-    <row r="100" spans="1:22">
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -4917,7 +3808,7 @@
       <c r="U100" s="1"/>
       <c r="V100" s="1"/>
     </row>
-    <row r="101" spans="1:22">
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -4941,7 +3832,7 @@
       <c r="U101" s="1"/>
       <c r="V101" s="1"/>
     </row>
-    <row r="102" spans="1:22">
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -4965,7 +3856,7 @@
       <c r="U102" s="1"/>
       <c r="V102" s="1"/>
     </row>
-    <row r="103" spans="1:22">
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -4989,7 +3880,7 @@
       <c r="U103" s="1"/>
       <c r="V103" s="1"/>
     </row>
-    <row r="104" spans="1:22">
+    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -5013,7 +3904,7 @@
       <c r="U104" s="1"/>
       <c r="V104" s="1"/>
     </row>
-    <row r="105" spans="1:22">
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -5037,7 +3928,7 @@
       <c r="U105" s="1"/>
       <c r="V105" s="1"/>
     </row>
-    <row r="106" spans="1:22">
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -5061,7 +3952,7 @@
       <c r="U106" s="1"/>
       <c r="V106" s="1"/>
     </row>
-    <row r="107" spans="1:22">
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -5085,7 +3976,7 @@
       <c r="U107" s="1"/>
       <c r="V107" s="1"/>
     </row>
-    <row r="108" spans="1:22">
+    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -5109,7 +4000,7 @@
       <c r="U108" s="1"/>
       <c r="V108" s="1"/>
     </row>
-    <row r="109" spans="1:22">
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -5133,7 +4024,7 @@
       <c r="U109" s="1"/>
       <c r="V109" s="1"/>
     </row>
-    <row r="110" spans="1:22">
+    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -5157,7 +4048,7 @@
       <c r="U110" s="1"/>
       <c r="V110" s="1"/>
     </row>
-    <row r="111" spans="1:22">
+    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -5181,7 +4072,7 @@
       <c r="U111" s="1"/>
       <c r="V111" s="1"/>
     </row>
-    <row r="112" spans="1:22">
+    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -5205,7 +4096,7 @@
       <c r="U112" s="1"/>
       <c r="V112" s="1"/>
     </row>
-    <row r="113" spans="1:22">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -5229,7 +4120,7 @@
       <c r="U113" s="1"/>
       <c r="V113" s="1"/>
     </row>
-    <row r="114" spans="1:22">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -5253,7 +4144,7 @@
       <c r="U114" s="1"/>
       <c r="V114" s="1"/>
     </row>
-    <row r="115" spans="1:22">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -5277,7 +4168,7 @@
       <c r="U115" s="1"/>
       <c r="V115" s="1"/>
     </row>
-    <row r="116" spans="1:22">
+    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -5301,7 +4192,7 @@
       <c r="U116" s="1"/>
       <c r="V116" s="1"/>
     </row>
-    <row r="117" spans="1:22">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -5325,7 +4216,7 @@
       <c r="U117" s="1"/>
       <c r="V117" s="1"/>
     </row>
-    <row r="118" spans="1:22">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -5349,7 +4240,7 @@
       <c r="U118" s="1"/>
       <c r="V118" s="1"/>
     </row>
-    <row r="119" spans="1:22">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -5373,7 +4264,7 @@
       <c r="U119" s="1"/>
       <c r="V119" s="1"/>
     </row>
-    <row r="120" spans="1:22">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -5397,7 +4288,7 @@
       <c r="U120" s="1"/>
       <c r="V120" s="1"/>
     </row>
-    <row r="121" spans="1:22">
+    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -5421,7 +4312,7 @@
       <c r="U121" s="1"/>
       <c r="V121" s="1"/>
     </row>
-    <row r="122" spans="1:22">
+    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -5445,7 +4336,7 @@
       <c r="U122" s="1"/>
       <c r="V122" s="1"/>
     </row>
-    <row r="123" spans="1:22">
+    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -5469,7 +4360,7 @@
       <c r="U123" s="1"/>
       <c r="V123" s="1"/>
     </row>
-    <row r="124" spans="1:22">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -5493,7 +4384,7 @@
       <c r="U124" s="1"/>
       <c r="V124" s="1"/>
     </row>
-    <row r="125" spans="1:22">
+    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -5517,7 +4408,7 @@
       <c r="U125" s="1"/>
       <c r="V125" s="1"/>
     </row>
-    <row r="126" spans="1:22">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -5541,7 +4432,7 @@
       <c r="U126" s="1"/>
       <c r="V126" s="1"/>
     </row>
-    <row r="127" spans="1:22">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -5565,7 +4456,7 @@
       <c r="U127" s="1"/>
       <c r="V127" s="1"/>
     </row>
-    <row r="128" spans="1:22">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -5589,7 +4480,7 @@
       <c r="U128" s="1"/>
       <c r="V128" s="1"/>
     </row>
-    <row r="129" spans="1:22">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -5613,7 +4504,7 @@
       <c r="U129" s="1"/>
       <c r="V129" s="1"/>
     </row>
-    <row r="130" spans="1:22">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -5637,7 +4528,7 @@
       <c r="U130" s="1"/>
       <c r="V130" s="1"/>
     </row>
-    <row r="131" spans="1:22">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -5661,7 +4552,7 @@
       <c r="U131" s="1"/>
       <c r="V131" s="1"/>
     </row>
-    <row r="132" spans="1:22">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -5685,7 +4576,7 @@
       <c r="U132" s="1"/>
       <c r="V132" s="1"/>
     </row>
-    <row r="133" spans="1:22">
+    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -5709,7 +4600,7 @@
       <c r="U133" s="1"/>
       <c r="V133" s="1"/>
     </row>
-    <row r="134" spans="1:22">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -5733,7 +4624,7 @@
       <c r="U134" s="1"/>
       <c r="V134" s="1"/>
     </row>
-    <row r="135" spans="1:22">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -5757,7 +4648,7 @@
       <c r="U135" s="1"/>
       <c r="V135" s="1"/>
     </row>
-    <row r="136" spans="1:22">
+    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -5781,7 +4672,7 @@
       <c r="U136" s="1"/>
       <c r="V136" s="1"/>
     </row>
-    <row r="137" spans="1:22">
+    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -5805,7 +4696,7 @@
       <c r="U137" s="1"/>
       <c r="V137" s="1"/>
     </row>
-    <row r="138" spans="1:22">
+    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -5829,7 +4720,7 @@
       <c r="U138" s="1"/>
       <c r="V138" s="1"/>
     </row>
-    <row r="139" spans="1:22">
+    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -5853,7 +4744,7 @@
       <c r="U139" s="1"/>
       <c r="V139" s="1"/>
     </row>
-    <row r="140" spans="1:22">
+    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -5877,7 +4768,7 @@
       <c r="U140" s="1"/>
       <c r="V140" s="1"/>
     </row>
-    <row r="141" spans="1:22">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -5901,7 +4792,7 @@
       <c r="U141" s="1"/>
       <c r="V141" s="1"/>
     </row>
-    <row r="142" spans="1:22">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -5925,7 +4816,7 @@
       <c r="U142" s="1"/>
       <c r="V142" s="1"/>
     </row>
-    <row r="143" spans="1:22">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -5949,7 +4840,7 @@
       <c r="U143" s="1"/>
       <c r="V143" s="1"/>
     </row>
-    <row r="144" spans="1:22">
+    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -5973,7 +4864,7 @@
       <c r="U144" s="1"/>
       <c r="V144" s="1"/>
     </row>
-    <row r="145" spans="1:22">
+    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -5997,7 +4888,7 @@
       <c r="U145" s="1"/>
       <c r="V145" s="1"/>
     </row>
-    <row r="146" spans="1:22">
+    <row r="146" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -6021,7 +4912,7 @@
       <c r="U146" s="1"/>
       <c r="V146" s="1"/>
     </row>
-    <row r="160" spans="1:22">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -6045,7 +4936,7 @@
       <c r="U160" s="1"/>
       <c r="V160" s="1"/>
     </row>
-    <row r="161" spans="1:22">
+    <row r="161" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -6069,7 +4960,7 @@
       <c r="U161" s="1"/>
       <c r="V161" s="1"/>
     </row>
-    <row r="162" spans="1:22">
+    <row r="162" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -6093,7 +4984,7 @@
       <c r="U162" s="1"/>
       <c r="V162" s="1"/>
     </row>
-    <row r="163" spans="1:22">
+    <row r="163" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -6117,7 +5008,7 @@
       <c r="U163" s="1"/>
       <c r="V163" s="1"/>
     </row>
-    <row r="164" spans="1:22">
+    <row r="164" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -6141,7 +5032,7 @@
       <c r="U164" s="1"/>
       <c r="V164" s="1"/>
     </row>
-    <row r="165" spans="1:22">
+    <row r="165" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -6165,7 +5056,7 @@
       <c r="U165" s="1"/>
       <c r="V165" s="1"/>
     </row>
-    <row r="166" spans="1:22">
+    <row r="166" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -6189,7 +5080,7 @@
       <c r="U166" s="1"/>
       <c r="V166" s="1"/>
     </row>
-    <row r="167" spans="1:22">
+    <row r="167" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -6213,7 +5104,7 @@
       <c r="U167" s="1"/>
       <c r="V167" s="1"/>
     </row>
-    <row r="168" spans="1:22">
+    <row r="168" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -6237,7 +5128,7 @@
       <c r="U168" s="1"/>
       <c r="V168" s="1"/>
     </row>
-    <row r="169" spans="1:22">
+    <row r="169" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -6261,7 +5152,7 @@
       <c r="U169" s="1"/>
       <c r="V169" s="1"/>
     </row>
-    <row r="170" spans="1:22">
+    <row r="170" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -6285,7 +5176,7 @@
       <c r="U170" s="1"/>
       <c r="V170" s="1"/>
     </row>
-    <row r="171" spans="1:22">
+    <row r="171" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -6309,7 +5200,7 @@
       <c r="U171" s="1"/>
       <c r="V171" s="1"/>
     </row>
-    <row r="172" spans="1:22">
+    <row r="172" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -6333,7 +5224,7 @@
       <c r="U172" s="1"/>
       <c r="V172" s="1"/>
     </row>
-    <row r="173" spans="1:22">
+    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -6357,7 +5248,7 @@
       <c r="U173" s="1"/>
       <c r="V173" s="1"/>
     </row>
-    <row r="174" spans="1:22">
+    <row r="174" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -6381,7 +5272,7 @@
       <c r="U174" s="1"/>
       <c r="V174" s="1"/>
     </row>
-    <row r="175" spans="1:22">
+    <row r="175" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>

</xml_diff>